<commit_message>
Created UPCB and PSU schematics, finalized BOM's
</commit_message>
<xml_diff>
--- a/Documentation/full_BOM.xlsx
+++ b/Documentation/full_BOM.xlsx
@@ -953,7 +953,7 @@
   <dimension ref="A1:P138"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2269,85 +2269,108 @@
     <hyperlink ref="G22" r:id="rId2" display="http://www.digikey.com/product-detail/en/ATMEGA328P-PN/ATMEGA328P-PN-ND/2357094"/>
     <hyperlink ref="E22" r:id="rId3" display="http://www.digikey.com/product-detail/en/ATMEGA328P-PN/ATMEGA328P-PN-ND/2357094"/>
     <hyperlink ref="D22" r:id="rId4" display="http://digikey.com/Suppliers/us/Atmel.page?lang=en"/>
-    <hyperlink ref="H34" r:id="rId5"/>
-    <hyperlink ref="G34" r:id="rId6" display="http://www.digikey.com/product-detail/en/2N3904TFR/2N3904D26ZCT-ND/458921"/>
-    <hyperlink ref="E34" r:id="rId7" display="http://www.digikey.com/product-detail/en/2N3904TFR/2N3904D26ZCT-ND/458921"/>
-    <hyperlink ref="D34" r:id="rId8" display="http://digikey.com/Suppliers/us/Fairchild-Semiconductor.page?lang=en"/>
-    <hyperlink ref="G33" r:id="rId9"/>
-    <hyperlink ref="H33" r:id="rId10"/>
-    <hyperlink ref="H29" r:id="rId11"/>
-    <hyperlink ref="H28" r:id="rId12"/>
-    <hyperlink ref="G29" r:id="rId13" display="http://www.digikey.com/product-detail/en/CF14JT10K0/CF14JT10K0CT-ND/1830374"/>
-    <hyperlink ref="E29" r:id="rId14" display="http://www.digikey.com/product-detail/en/CF14JT10K0/CF14JT10K0CT-ND/1830374"/>
-    <hyperlink ref="D29" r:id="rId15" display="http://digikey.com/Suppliers/us/Stackpole-Electronics.page?lang=en"/>
-    <hyperlink ref="G28" r:id="rId16" display="http://www.digikey.com/product-detail/en/CF14JT220R/CF14JT220RCT-ND/1830334"/>
-    <hyperlink ref="E28" r:id="rId17" display="http://www.digikey.com/product-detail/en/CF14JT220R/CF14JT220RCT-ND/1830334"/>
-    <hyperlink ref="D28" r:id="rId18" display="http://digikey.com/Suppliers/us/Stackpole-Electronics.page?lang=en"/>
-    <hyperlink ref="H9" r:id="rId19"/>
-    <hyperlink ref="G9" r:id="rId20" display="http://www.digikey.com/product-detail/en/ATS16B/CTX1085-ND/2640031"/>
-    <hyperlink ref="E9" r:id="rId21" display="http://www.digikey.com/product-detail/en/ATS16B/CTX1085-ND/2640031"/>
-    <hyperlink ref="D9" r:id="rId22" display="http://digikey.com/Suppliers/us/CTS-Frequency-Controls.page?lang=en"/>
-    <hyperlink ref="H21" r:id="rId23"/>
-    <hyperlink ref="G21" r:id="rId24" display="http://www.digikey.com/product-detail/en/TLHR4405/751-1129-ND/1681264"/>
-    <hyperlink ref="E21" r:id="rId25" display="http://www.digikey.com/product-detail/en/TLHR4405/751-1129-ND/1681264"/>
-    <hyperlink ref="D21" r:id="rId26" display="http://digikey.com/Suppliers/us/Vishay-Semiconductors.page?lang=en"/>
-    <hyperlink ref="E13" r:id="rId27" display="http://www.digikey.com/product-detail/en/SN74LS14NSR/296-3652-1-ND/377690"/>
-    <hyperlink ref="G13" r:id="rId28" display="http://www.digikey.com/product-detail/en/SN74LS14NSR/296-3652-1-ND/377690"/>
-    <hyperlink ref="D13" r:id="rId29" display="http://digikey.com/Suppliers/us/Texas-Instruments.page?lang=en"/>
-    <hyperlink ref="G6" r:id="rId30" display="http://www.digikey.com/product-detail/en/EEU-FR1A101B/P15316CT-ND/3072196"/>
-    <hyperlink ref="E6" r:id="rId31" display="http://www.digikey.com/product-detail/en/EEU-FR1A101B/P15316CT-ND/3072196"/>
-    <hyperlink ref="H7" r:id="rId32"/>
-    <hyperlink ref="D6" r:id="rId33" display="http://digikey.com/Suppliers/us/Panasonic-Electronic-Components.page?lang=en"/>
-    <hyperlink ref="G7" r:id="rId34" display="http://www.digikey.com/product-detail/en/FK18X7R1H104K/445-5303-ND/2256783"/>
-    <hyperlink ref="E7" r:id="rId35" display="http://www.digikey.com/product-detail/en/FK18X7R1H104K/445-5303-ND/2256783"/>
-    <hyperlink ref="D7" r:id="rId36" display="http://digikey.com/Suppliers/us/TDK.page?lang=en"/>
-    <hyperlink ref="G5" r:id="rId37" display="http://www.digikey.com/product-detail/en/FK28C0G1H220J/445-4718-ND/2050067"/>
-    <hyperlink ref="E5" r:id="rId38" display="http://www.digikey.com/product-detail/en/FK28C0G1H220J/445-4718-ND/2050067"/>
-    <hyperlink ref="D5" r:id="rId39" display="http://digikey.com/Suppliers/us/TDK.page?lang=en"/>
-    <hyperlink ref="H35" r:id="rId40"/>
-    <hyperlink ref="H36" r:id="rId41"/>
-    <hyperlink ref="G36" r:id="rId42"/>
-    <hyperlink ref="G35" r:id="rId43"/>
-    <hyperlink ref="G30" r:id="rId44"/>
-    <hyperlink ref="G31" r:id="rId45"/>
-    <hyperlink ref="G25" r:id="rId46" display="http://www.frys.com/product/4986181?source=googleps&amp;gclid=CNPX5OnlxbQCFcxAMgodfm0AYw"/>
-    <hyperlink ref="G2" r:id="rId47"/>
-    <hyperlink ref="G17" r:id="rId48"/>
-    <hyperlink ref="H8" r:id="rId49"/>
-    <hyperlink ref="G8" r:id="rId50"/>
-    <hyperlink ref="G23" r:id="rId51"/>
-    <hyperlink ref="G3" r:id="rId52"/>
-    <hyperlink ref="G26" r:id="rId53"/>
-    <hyperlink ref="G4" r:id="rId54"/>
-    <hyperlink ref="G14" r:id="rId55"/>
-    <hyperlink ref="G16" r:id="rId56"/>
-    <hyperlink ref="G32" r:id="rId57"/>
-    <hyperlink ref="G24" r:id="rId58" display="http://www.adafruit.com/products/572"/>
-    <hyperlink ref="G27" r:id="rId59"/>
-    <hyperlink ref="D10" r:id="rId60" display="http://digikey.com/Suppliers/us/Molex.page?lang=en"/>
-    <hyperlink ref="E10" r:id="rId61" display="http://www.digikey.com/product-detail/en/0022232031/WM4201-ND/26669"/>
-    <hyperlink ref="G10" r:id="rId62" display="http://www.digikey.com/product-detail/en/0022232031/WM4201-ND/26669"/>
-    <hyperlink ref="D11" r:id="rId63" display="http://digikey.com/Suppliers/us/Molex.page?lang=en"/>
-    <hyperlink ref="E11" r:id="rId64" display="http://www.digikey.com/product-detail/en/0022232051/WM4203-ND/26673"/>
-    <hyperlink ref="G11" r:id="rId65" display="http://www.digikey.com/product-detail/en/0022232051/WM4203-ND/26673"/>
-    <hyperlink ref="H11" r:id="rId66"/>
-    <hyperlink ref="E12" r:id="rId67" display="http://www.digikey.com/product-detail/en/0022232021/WM4200-ND/26667"/>
-    <hyperlink ref="D12" r:id="rId68" display="http://digikey.com/Suppliers/us/Molex.page?lang=en"/>
-    <hyperlink ref="G12" r:id="rId69" display="http://www.digikey.com/product-detail/en/0022232021/WM4200-ND/26667"/>
-    <hyperlink ref="D20" r:id="rId70" display="http://digikey.com/Suppliers/us/Molex.page?lang=en"/>
-    <hyperlink ref="G20" r:id="rId71"/>
-    <hyperlink ref="E20" r:id="rId72" display="http://www.digikey.com/scripts/dksearch/dksus.dll?vendor=0&amp;keywords=22-01-2057"/>
-    <hyperlink ref="D19" r:id="rId73" display="http://digikey.com/Suppliers/us/Molex.page?lang=en"/>
-    <hyperlink ref="E19" r:id="rId74" display="http://www.digikey.com/product-detail/en/0022012027/WM2011-ND/171991"/>
-    <hyperlink ref="G19" r:id="rId75" display="http://www.digikey.com/product-detail/en/0022012027/WM2011-ND/171991"/>
-    <hyperlink ref="D18" r:id="rId76" display="http://digikey.com/Suppliers/us/Molex.page?lang=en"/>
-    <hyperlink ref="E18" r:id="rId77" display="http://www.digikey.com/product-detail/en/0022012037/WM2012-ND/171992"/>
-    <hyperlink ref="G18" r:id="rId78" display="http://www.digikey.com/product-detail/en/0022012037/WM2012-ND/171992"/>
+    <hyperlink ref="G34" r:id="rId5" display="http://www.digikey.com/product-detail/en/2N3904TFR/2N3904D26ZCT-ND/458921"/>
+    <hyperlink ref="E34" r:id="rId6" display="http://www.digikey.com/product-detail/en/2N3904TFR/2N3904D26ZCT-ND/458921"/>
+    <hyperlink ref="D34" r:id="rId7" display="http://digikey.com/Suppliers/us/Fairchild-Semiconductor.page?lang=en"/>
+    <hyperlink ref="G33" r:id="rId8"/>
+    <hyperlink ref="H33" r:id="rId9"/>
+    <hyperlink ref="H29" r:id="rId10"/>
+    <hyperlink ref="H28" r:id="rId11"/>
+    <hyperlink ref="G29" r:id="rId12" display="http://www.digikey.com/product-detail/en/CF14JT10K0/CF14JT10K0CT-ND/1830374"/>
+    <hyperlink ref="E29" r:id="rId13" display="http://www.digikey.com/product-detail/en/CF14JT10K0/CF14JT10K0CT-ND/1830374"/>
+    <hyperlink ref="D29" r:id="rId14" display="http://digikey.com/Suppliers/us/Stackpole-Electronics.page?lang=en"/>
+    <hyperlink ref="G28" r:id="rId15" display="http://www.digikey.com/product-detail/en/CF14JT220R/CF14JT220RCT-ND/1830334"/>
+    <hyperlink ref="E28" r:id="rId16" display="http://www.digikey.com/product-detail/en/CF14JT220R/CF14JT220RCT-ND/1830334"/>
+    <hyperlink ref="D28" r:id="rId17" display="http://digikey.com/Suppliers/us/Stackpole-Electronics.page?lang=en"/>
+    <hyperlink ref="H9" r:id="rId18"/>
+    <hyperlink ref="G9" r:id="rId19" display="http://www.digikey.com/product-detail/en/ATS16B/CTX1085-ND/2640031"/>
+    <hyperlink ref="E9" r:id="rId20" display="http://www.digikey.com/product-detail/en/ATS16B/CTX1085-ND/2640031"/>
+    <hyperlink ref="D9" r:id="rId21" display="http://digikey.com/Suppliers/us/CTS-Frequency-Controls.page?lang=en"/>
+    <hyperlink ref="H21" r:id="rId22"/>
+    <hyperlink ref="G21" r:id="rId23" display="http://www.digikey.com/product-detail/en/TLHR4405/751-1129-ND/1681264"/>
+    <hyperlink ref="E21" r:id="rId24" display="http://www.digikey.com/product-detail/en/TLHR4405/751-1129-ND/1681264"/>
+    <hyperlink ref="D21" r:id="rId25" display="http://digikey.com/Suppliers/us/Vishay-Semiconductors.page?lang=en"/>
+    <hyperlink ref="E13" r:id="rId26" display="http://www.digikey.com/product-detail/en/SN74LS14NSR/296-3652-1-ND/377690"/>
+    <hyperlink ref="G13" r:id="rId27" display="http://www.digikey.com/product-detail/en/SN74LS14NSR/296-3652-1-ND/377690"/>
+    <hyperlink ref="D13" r:id="rId28" display="http://digikey.com/Suppliers/us/Texas-Instruments.page?lang=en"/>
+    <hyperlink ref="G6" r:id="rId29" display="http://www.digikey.com/product-detail/en/EEU-FR1A101B/P15316CT-ND/3072196"/>
+    <hyperlink ref="E6" r:id="rId30" display="http://www.digikey.com/product-detail/en/EEU-FR1A101B/P15316CT-ND/3072196"/>
+    <hyperlink ref="H7" r:id="rId31"/>
+    <hyperlink ref="D6" r:id="rId32" display="http://digikey.com/Suppliers/us/Panasonic-Electronic-Components.page?lang=en"/>
+    <hyperlink ref="G7" r:id="rId33" display="http://www.digikey.com/product-detail/en/FK18X7R1H104K/445-5303-ND/2256783"/>
+    <hyperlink ref="E7" r:id="rId34" display="http://www.digikey.com/product-detail/en/FK18X7R1H104K/445-5303-ND/2256783"/>
+    <hyperlink ref="D7" r:id="rId35" display="http://digikey.com/Suppliers/us/TDK.page?lang=en"/>
+    <hyperlink ref="G5" r:id="rId36" display="http://www.digikey.com/product-detail/en/FK28C0G1H220J/445-4718-ND/2050067"/>
+    <hyperlink ref="E5" r:id="rId37" display="http://www.digikey.com/product-detail/en/FK28C0G1H220J/445-4718-ND/2050067"/>
+    <hyperlink ref="D5" r:id="rId38" display="http://digikey.com/Suppliers/us/TDK.page?lang=en"/>
+    <hyperlink ref="G36" r:id="rId39"/>
+    <hyperlink ref="G35" r:id="rId40"/>
+    <hyperlink ref="G30" r:id="rId41"/>
+    <hyperlink ref="G31" r:id="rId42"/>
+    <hyperlink ref="G25" r:id="rId43" display="http://www.frys.com/product/4986181?source=googleps&amp;gclid=CNPX5OnlxbQCFcxAMgodfm0AYw"/>
+    <hyperlink ref="G2" r:id="rId44"/>
+    <hyperlink ref="G17" r:id="rId45"/>
+    <hyperlink ref="H8" r:id="rId46"/>
+    <hyperlink ref="G8" r:id="rId47"/>
+    <hyperlink ref="G23" r:id="rId48"/>
+    <hyperlink ref="G3" r:id="rId49"/>
+    <hyperlink ref="G26" r:id="rId50"/>
+    <hyperlink ref="G4" r:id="rId51"/>
+    <hyperlink ref="G14" r:id="rId52"/>
+    <hyperlink ref="G16" r:id="rId53"/>
+    <hyperlink ref="G32" r:id="rId54"/>
+    <hyperlink ref="G24" r:id="rId55" display="http://www.adafruit.com/products/572"/>
+    <hyperlink ref="G27" r:id="rId56"/>
+    <hyperlink ref="D10" r:id="rId57" display="http://digikey.com/Suppliers/us/Molex.page?lang=en"/>
+    <hyperlink ref="E10" r:id="rId58" display="http://www.digikey.com/product-detail/en/0022232031/WM4201-ND/26669"/>
+    <hyperlink ref="G10" r:id="rId59" display="http://www.digikey.com/product-detail/en/0022232031/WM4201-ND/26669"/>
+    <hyperlink ref="D11" r:id="rId60" display="http://digikey.com/Suppliers/us/Molex.page?lang=en"/>
+    <hyperlink ref="E11" r:id="rId61" display="http://www.digikey.com/product-detail/en/0022232051/WM4203-ND/26673"/>
+    <hyperlink ref="G11" r:id="rId62" display="http://www.digikey.com/product-detail/en/0022232051/WM4203-ND/26673"/>
+    <hyperlink ref="H11" r:id="rId63"/>
+    <hyperlink ref="E12" r:id="rId64" display="http://www.digikey.com/product-detail/en/0022232021/WM4200-ND/26667"/>
+    <hyperlink ref="D12" r:id="rId65" display="http://digikey.com/Suppliers/us/Molex.page?lang=en"/>
+    <hyperlink ref="G12" r:id="rId66" display="http://www.digikey.com/product-detail/en/0022232021/WM4200-ND/26667"/>
+    <hyperlink ref="D20" r:id="rId67" display="http://digikey.com/Suppliers/us/Molex.page?lang=en"/>
+    <hyperlink ref="G20" r:id="rId68"/>
+    <hyperlink ref="E20" r:id="rId69" display="http://www.digikey.com/scripts/dksearch/dksus.dll?vendor=0&amp;keywords=22-01-2057"/>
+    <hyperlink ref="D19" r:id="rId70" display="http://digikey.com/Suppliers/us/Molex.page?lang=en"/>
+    <hyperlink ref="E19" r:id="rId71" display="http://www.digikey.com/product-detail/en/0022012027/WM2011-ND/171991"/>
+    <hyperlink ref="G19" r:id="rId72" display="http://www.digikey.com/product-detail/en/0022012027/WM2011-ND/171991"/>
+    <hyperlink ref="D18" r:id="rId73" display="http://digikey.com/Suppliers/us/Molex.page?lang=en"/>
+    <hyperlink ref="E18" r:id="rId74" display="http://www.digikey.com/product-detail/en/0022012037/WM2012-ND/171992"/>
+    <hyperlink ref="G18" r:id="rId75" display="http://www.digikey.com/product-detail/en/0022012037/WM2012-ND/171992"/>
+    <hyperlink ref="H2" r:id="rId76"/>
+    <hyperlink ref="H3" r:id="rId77"/>
+    <hyperlink ref="H4" r:id="rId78"/>
+    <hyperlink ref="H5" r:id="rId79"/>
+    <hyperlink ref="H6" r:id="rId80"/>
+    <hyperlink ref="H10" r:id="rId81"/>
+    <hyperlink ref="H12" r:id="rId82"/>
+    <hyperlink ref="H13" r:id="rId83"/>
+    <hyperlink ref="H14" r:id="rId84"/>
+    <hyperlink ref="H15" r:id="rId85"/>
+    <hyperlink ref="H16" r:id="rId86"/>
+    <hyperlink ref="H17" r:id="rId87"/>
+    <hyperlink ref="H18" r:id="rId88"/>
+    <hyperlink ref="H19" r:id="rId89"/>
+    <hyperlink ref="H20" r:id="rId90"/>
+    <hyperlink ref="H23" r:id="rId91"/>
+    <hyperlink ref="H24" r:id="rId92"/>
+    <hyperlink ref="H25" r:id="rId93"/>
+    <hyperlink ref="H26" r:id="rId94"/>
+    <hyperlink ref="H27" r:id="rId95"/>
+    <hyperlink ref="H30" r:id="rId96"/>
+    <hyperlink ref="H31" r:id="rId97"/>
+    <hyperlink ref="H32" r:id="rId98"/>
+    <hyperlink ref="H34" r:id="rId99"/>
+    <hyperlink ref="H35" r:id="rId100"/>
+    <hyperlink ref="H36" r:id="rId101"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="46" orientation="landscape" r:id="rId79"/>
+  <pageSetup scale="46" orientation="landscape" r:id="rId102"/>
   <tableParts count="1">
-    <tablePart r:id="rId80"/>
+    <tablePart r:id="rId103"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>